<commit_message>
first version of archetypes consumptions
</commit_message>
<xml_diff>
--- a/dev/write_files/comparison_total_demands.xlsx
+++ b/dev/write_files/comparison_total_demands.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t>Froemelt</t>
   </si>
@@ -23,12 +23,6 @@
   </si>
   <si>
     <t>HABE 091011 / Froemelt</t>
-  </si>
-  <si>
-    <t>HABE 151617</t>
-  </si>
-  <si>
-    <t>HABE 151617 / Froemelt</t>
   </si>
   <si>
     <t>Other insurance premiums</t>
@@ -995,13 +989,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F204"/>
+  <dimension ref="A1:D204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,16 +1005,10 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B2">
         <v>1961093.91327612</v>
@@ -1031,16 +1019,10 @@
       <c r="D2">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E2">
-        <v>1968236.287353748</v>
-      </c>
-      <c r="F2">
-        <v>1.003642035717553</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>745048.1685118984</v>
@@ -1051,16 +1033,10 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>747854.0242940877</v>
-      </c>
-      <c r="F3">
-        <v>1.003766005878242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>448103.1234104093</v>
@@ -1071,16 +1047,10 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>441284.9810245644</v>
-      </c>
-      <c r="F4">
-        <v>0.9847844345873923</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>28832.4549974995</v>
@@ -1091,16 +1061,10 @@
       <c r="D5">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E5">
-        <v>46228.0191056988</v>
-      </c>
-      <c r="F5">
-        <v>1.603332741166436</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>88865.51031371718</v>
@@ -1111,16 +1075,10 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>93385.69988874221</v>
-      </c>
-      <c r="F6">
-        <v>1.050865510804671</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>8691.4424022884</v>
@@ -1131,16 +1089,10 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>10230.2192901335</v>
-      </c>
-      <c r="F7">
-        <v>1.177045053815228</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>19039.2275618517</v>
@@ -1151,16 +1103,10 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>22043.4551485189</v>
-      </c>
-      <c r="F8">
-        <v>1.15779146380322</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>58708.2700442855</v>
@@ -1171,16 +1117,10 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>52723.8295175754</v>
-      </c>
-      <c r="F9">
-        <v>0.8980647782297819</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>6951.2652302493</v>
@@ -1191,16 +1131,10 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>7365.826304202499</v>
-      </c>
-      <c r="F10">
-        <v>1.059638218399319</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>132559.7181839645</v>
@@ -1211,16 +1145,10 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11">
-        <v>128043.6638886072</v>
-      </c>
-      <c r="F11">
-        <v>0.965931925948349</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>39970.9331253195</v>
@@ -1231,16 +1159,10 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>32878.5229598662</v>
-      </c>
-      <c r="F12">
-        <v>0.822560805793132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>121085.236855309</v>
@@ -1251,16 +1173,10 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>125076.0358023553</v>
-      </c>
-      <c r="F13">
-        <v>1.032958592233792</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>7213.513560747801</v>
@@ -1271,16 +1187,10 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>11340.2106605912</v>
-      </c>
-      <c r="F14">
-        <v>1.572078650035226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>354306.4719774659</v>
@@ -1291,16 +1201,10 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>343881.905991014</v>
-      </c>
-      <c r="F15">
-        <v>0.9705775456816523</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>2959832.855808329</v>
@@ -1311,16 +1215,10 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>3166781.439384385</v>
-      </c>
-      <c r="F16">
-        <v>1.069919010179897</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>680809.8712559623</v>
@@ -1331,16 +1229,10 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17">
-        <v>715788.1159910313</v>
-      </c>
-      <c r="F17">
-        <v>1.051377405369492</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>394895.2214092204</v>
@@ -1351,16 +1243,10 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18">
-        <v>348286.885881145</v>
-      </c>
-      <c r="F18">
-        <v>0.8819729057197776</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>889400.8270847967</v>
@@ -1371,16 +1257,10 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19">
-        <v>1123807.10578483</v>
-      </c>
-      <c r="F19">
-        <v>1.263555274024593</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>12450.0291809752</v>
@@ -1391,16 +1271,10 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20">
-        <v>11626.2418342896</v>
-      </c>
-      <c r="F20">
-        <v>0.9338324967186082</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>554938.5119814473</v>
@@ -1411,16 +1285,10 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21">
-        <v>489567.9374786669</v>
-      </c>
-      <c r="F21">
-        <v>0.8822021303416658</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>1010289.935069157</v>
@@ -1431,16 +1299,10 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22">
-        <v>919948.9211597614</v>
-      </c>
-      <c r="F22">
-        <v>0.9105791211280241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>204836.5199297618</v>
@@ -1451,16 +1313,10 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23">
-        <v>191481.7621229989</v>
-      </c>
-      <c r="F23">
-        <v>0.9348028476008955</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>85068.5846832122</v>
@@ -1471,16 +1327,10 @@
       <c r="D24">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E24">
-        <v>71697.4244746636</v>
-      </c>
-      <c r="F24">
-        <v>0.8428190587824916</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>21180.9125113228</v>
@@ -1491,16 +1341,10 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25">
-        <v>18142.3455501066</v>
-      </c>
-      <c r="F25">
-        <v>0.8565422070653539</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>50910.3681026141</v>
@@ -1511,16 +1355,10 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26">
-        <v>50711.6546976301</v>
-      </c>
-      <c r="F26">
-        <v>0.9960967988959838</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>139848.3872855041</v>
@@ -1531,16 +1369,10 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27">
-        <v>133738.9744083633</v>
-      </c>
-      <c r="F27">
-        <v>0.9563140269564334</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>241457.9289617749</v>
@@ -1551,16 +1383,10 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28">
-        <v>226396.4183589932</v>
-      </c>
-      <c r="F28">
-        <v>0.9376226298819698</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>73082.1293310926</v>
@@ -1571,16 +1397,10 @@
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29">
-        <v>71261.48779865079</v>
-      </c>
-      <c r="F29">
-        <v>0.9750877328136741</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>16417.8173131013</v>
@@ -1591,16 +1411,10 @@
       <c r="D30">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E30">
-        <v>12305.0542246733</v>
-      </c>
-      <c r="F30">
-        <v>0.749493918101644</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>261891.6231343206</v>
@@ -1611,16 +1425,10 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31">
-        <v>331560.11380696</v>
-      </c>
-      <c r="F31">
-        <v>1.266020309618332</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>814140.6762847268</v>
@@ -1631,16 +1439,10 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32">
-        <v>766536.672803849</v>
-      </c>
-      <c r="F32">
-        <v>0.9415285283397025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>1131067.085941838</v>
@@ -1651,16 +1453,10 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33">
-        <v>838989.7428099304</v>
-      </c>
-      <c r="F33">
-        <v>0.7417683294278737</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>280817.9678889848</v>
@@ -1671,16 +1467,10 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34">
-        <v>268748.2628122356</v>
-      </c>
-      <c r="F34">
-        <v>0.957019470059264</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>172838.180490952</v>
@@ -1691,16 +1481,10 @@
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35">
-        <v>130554.058960505</v>
-      </c>
-      <c r="F35">
-        <v>0.7553542775656532</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>130178.1458214003</v>
@@ -1711,16 +1495,10 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36">
-        <v>133987.1163086073</v>
-      </c>
-      <c r="F36">
-        <v>1.029259676907926</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>94202.2699279333</v>
@@ -1731,16 +1509,10 @@
       <c r="D37">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E37">
-        <v>87847.9104198436</v>
-      </c>
-      <c r="F37">
-        <v>0.9325455797089505</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>32880.1268067027</v>
@@ -1751,16 +1523,10 @@
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38">
-        <v>20508.9375890005</v>
-      </c>
-      <c r="F38">
-        <v>0.6237487376362459</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>57813.570429679</v>
@@ -1771,16 +1537,10 @@
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39">
-        <v>48048.5045384407</v>
-      </c>
-      <c r="F39">
-        <v>0.8310938795396499</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>10828.6215190113</v>
@@ -1791,16 +1551,10 @@
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40">
-        <v>8502.296905943402</v>
-      </c>
-      <c r="F40">
-        <v>0.7851689054803809</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>93534.5120319183</v>
@@ -1811,16 +1565,10 @@
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="E41">
-        <v>89779.0205070864</v>
-      </c>
-      <c r="F41">
-        <v>0.9598491354340913</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>44249.0136013317</v>
@@ -1831,16 +1579,10 @@
       <c r="D42">
         <v>1</v>
       </c>
-      <c r="E42">
-        <v>44660.1321435945</v>
-      </c>
-      <c r="F42">
-        <v>1.009291021625179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>292495.2139409842</v>
@@ -1851,16 +1593,10 @@
       <c r="D43">
         <v>1</v>
       </c>
-      <c r="E43">
-        <v>206962.4157630821</v>
-      </c>
-      <c r="F43">
-        <v>0.707575392344164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>75422.45449794231</v>
@@ -1871,16 +1607,10 @@
       <c r="D44">
         <v>1</v>
       </c>
-      <c r="E44">
-        <v>68671.8787416102</v>
-      </c>
-      <c r="F44">
-        <v>0.9104964721545057</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>203351.4241544241</v>
@@ -1891,16 +1621,10 @@
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="E45">
-        <v>180345.6528379317</v>
-      </c>
-      <c r="F45">
-        <v>0.8868669279688843</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>12155.2185675531</v>
@@ -1911,16 +1635,10 @@
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="E46">
-        <v>12821.1332364766</v>
-      </c>
-      <c r="F46">
-        <v>1.054784261197991</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B47">
         <v>5176.985398519901</v>
@@ -1931,16 +1649,10 @@
       <c r="D47">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E47">
-        <v>3953.2896268515</v>
-      </c>
-      <c r="F47">
-        <v>0.7636277336192111</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <v>135149.3155498248</v>
@@ -1951,16 +1663,10 @@
       <c r="D48">
         <v>1</v>
       </c>
-      <c r="E48">
-        <v>125760.289934647</v>
-      </c>
-      <c r="F48">
-        <v>0.9305285004442631</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <v>172795.4508208</v>
@@ -1971,16 +1677,10 @@
       <c r="D49">
         <v>1</v>
       </c>
-      <c r="E49">
-        <v>167393.0071987659</v>
-      </c>
-      <c r="F49">
-        <v>0.9687350355789356</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>397372.9124656621</v>
@@ -1991,16 +1691,10 @@
       <c r="D50">
         <v>1</v>
       </c>
-      <c r="E50">
-        <v>402911.0756446033</v>
-      </c>
-      <c r="F50">
-        <v>1.01393694186294</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>273986.7851446504</v>
@@ -2011,16 +1705,10 @@
       <c r="D51">
         <v>1</v>
       </c>
-      <c r="E51">
-        <v>239715.9159010448</v>
-      </c>
-      <c r="F51">
-        <v>0.8749178022381174</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>77578.30881480001</v>
@@ -2031,16 +1719,10 @@
       <c r="D52">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E52">
-        <v>107629.8576308929</v>
-      </c>
-      <c r="F52">
-        <v>1.387370506978103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>2025526.499779646</v>
@@ -2051,16 +1733,10 @@
       <c r="D53">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E53">
-        <v>1868471.379898388</v>
-      </c>
-      <c r="F53">
-        <v>0.9224620759598336</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>132713.509867926</v>
@@ -2071,16 +1747,10 @@
       <c r="D54">
         <v>1</v>
       </c>
-      <c r="E54">
-        <v>123649.2885512875</v>
-      </c>
-      <c r="F54">
-        <v>0.9317008394574218</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B55">
         <v>284808.3262732538</v>
@@ -2091,16 +1761,10 @@
       <c r="D55">
         <v>1</v>
       </c>
-      <c r="E55">
-        <v>247560.056207533</v>
-      </c>
-      <c r="F55">
-        <v>0.8692163584080627</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B56">
         <v>21151.2369171201</v>
@@ -2111,16 +1775,10 @@
       <c r="D56">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E56">
-        <v>12689.9717811844</v>
-      </c>
-      <c r="F56">
-        <v>0.5999635780597287</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B57">
         <v>54527.47692874441</v>
@@ -2131,16 +1789,10 @@
       <c r="D57">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E57">
-        <v>39375.7272648439</v>
-      </c>
-      <c r="F57">
-        <v>0.7221263385485348</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>31969.342329154</v>
@@ -2151,16 +1803,10 @@
       <c r="D58">
         <v>1</v>
       </c>
-      <c r="E58">
-        <v>38711.5409399511</v>
-      </c>
-      <c r="F58">
-        <v>1.210895755733099</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>318381.0785552047</v>
@@ -2171,16 +1817,10 @@
       <c r="D59">
         <v>1</v>
       </c>
-      <c r="E59">
-        <v>435670.7411449056</v>
-      </c>
-      <c r="F59">
-        <v>1.36839394828975</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>49163.0630633078</v>
@@ -2191,16 +1831,10 @@
       <c r="D60">
         <v>1</v>
       </c>
-      <c r="E60">
-        <v>21723.1098729114</v>
-      </c>
-      <c r="F60">
-        <v>0.4418583489181364</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B61">
         <v>37507.6760315389</v>
@@ -2211,16 +1845,10 @@
       <c r="D61">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E61">
-        <v>44287.8381209504</v>
-      </c>
-      <c r="F61">
-        <v>1.180767320366911</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B62">
         <v>55957.8486221378</v>
@@ -2231,16 +1859,10 @@
       <c r="D62">
         <v>1</v>
       </c>
-      <c r="E62">
-        <v>48565.6385756252</v>
-      </c>
-      <c r="F62">
-        <v>0.8678968146822549</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B63">
         <v>77465.0976228716</v>
@@ -2251,16 +1873,10 @@
       <c r="D63">
         <v>1</v>
       </c>
-      <c r="E63">
-        <v>117384.1769942627</v>
-      </c>
-      <c r="F63">
-        <v>1.515316969788533</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>656518.4260099236</v>
@@ -2271,16 +1887,10 @@
       <c r="D64">
         <v>1</v>
       </c>
-      <c r="E64">
-        <v>867628.2921496774</v>
-      </c>
-      <c r="F64">
-        <v>1.321559696995561</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <v>632047.2423178807</v>
@@ -2291,16 +1901,10 @@
       <c r="D65">
         <v>1</v>
       </c>
-      <c r="E65">
-        <v>775679.4965853564</v>
-      </c>
-      <c r="F65">
-        <v>1.227249238111916</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <v>291810.7921287232</v>
@@ -2311,16 +1915,10 @@
       <c r="D66">
         <v>1</v>
       </c>
-      <c r="E66">
-        <v>47999.8751072604</v>
-      </c>
-      <c r="F66">
-        <v>0.1644897186876035</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>312405.08405326</v>
@@ -2331,16 +1929,10 @@
       <c r="D67">
         <v>1</v>
       </c>
-      <c r="E67">
-        <v>161561.256341342</v>
-      </c>
-      <c r="F67">
-        <v>0.5171530957345062</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B68">
         <v>86266.8170776265</v>
@@ -2351,16 +1943,10 @@
       <c r="D68">
         <v>1</v>
       </c>
-      <c r="E68">
-        <v>61961.77624620761</v>
-      </c>
-      <c r="F68">
-        <v>0.7182573594949239</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B69">
         <v>120147.0270680439</v>
@@ -2371,16 +1957,10 @@
       <c r="D69">
         <v>1</v>
       </c>
-      <c r="E69">
-        <v>58416.3266946846</v>
-      </c>
-      <c r="F69">
-        <v>0.4862070091971662</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B70">
         <v>201973.1255670026</v>
@@ -2391,16 +1971,10 @@
       <c r="D70">
         <v>1</v>
       </c>
-      <c r="E70">
-        <v>189712.2157763581</v>
-      </c>
-      <c r="F70">
-        <v>0.9392943503932802</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B71">
         <v>268414.705830991</v>
@@ -2411,16 +1985,10 @@
       <c r="D71">
         <v>1</v>
       </c>
-      <c r="E71">
-        <v>213056.8022070994</v>
-      </c>
-      <c r="F71">
-        <v>0.7937597962357993</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B72">
         <v>222044.9265093554</v>
@@ -2431,16 +1999,10 @@
       <c r="D72">
         <v>1</v>
       </c>
-      <c r="E72">
-        <v>189706.751567419</v>
-      </c>
-      <c r="F72">
-        <v>0.8543620183072552</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B73">
         <v>340134.844628405</v>
@@ -2451,16 +2013,10 @@
       <c r="D73">
         <v>1</v>
       </c>
-      <c r="E73">
-        <v>300389.7373503538</v>
-      </c>
-      <c r="F73">
-        <v>0.88314896898766</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B74">
         <v>209772.6226962424</v>
@@ -2471,16 +2027,10 @@
       <c r="D74">
         <v>1</v>
       </c>
-      <c r="E74">
-        <v>192680.2566124762</v>
-      </c>
-      <c r="F74">
-        <v>0.9185195576807155</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B75">
         <v>144997.9075514856</v>
@@ -2491,16 +2041,10 @@
       <c r="D75">
         <v>1</v>
       </c>
-      <c r="E75">
-        <v>121699.4779827154</v>
-      </c>
-      <c r="F75">
-        <v>0.8393188566497248</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>35959.7986976075</v>
@@ -2511,16 +2055,10 @@
       <c r="D76">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E76">
-        <v>35679.9094304049</v>
-      </c>
-      <c r="F76">
-        <v>0.992216606395485</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B77">
         <v>283149.6494303539</v>
@@ -2531,16 +2069,10 @@
       <c r="D77">
         <v>1</v>
       </c>
-      <c r="E77">
-        <v>349530.5986426391</v>
-      </c>
-      <c r="F77">
-        <v>1.234437688147705</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>123023.4271935566</v>
@@ -2551,16 +2083,10 @@
       <c r="D78">
         <v>1</v>
       </c>
-      <c r="E78">
-        <v>125674.3674430833</v>
-      </c>
-      <c r="F78">
-        <v>1.021548255564007</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B79">
         <v>46868.1261450503</v>
@@ -2571,16 +2097,10 @@
       <c r="D79">
         <v>1</v>
       </c>
-      <c r="E79">
-        <v>55527.9327501654</v>
-      </c>
-      <c r="F79">
-        <v>1.184769635942222</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B80">
         <v>138373.6485454249</v>
@@ -2591,16 +2111,10 @@
       <c r="D80">
         <v>1</v>
       </c>
-      <c r="E80">
-        <v>162603.2272527888</v>
-      </c>
-      <c r="F80">
-        <v>1.175102549958491</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B81">
         <v>132169.5803060309</v>
@@ -2611,16 +2125,10 @@
       <c r="D81">
         <v>1</v>
       </c>
-      <c r="E81">
-        <v>128687.5540645887</v>
-      </c>
-      <c r="F81">
-        <v>0.9736548589064157</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B82">
         <v>75709.86029758392</v>
@@ -2631,16 +2139,10 @@
       <c r="D82">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E82">
-        <v>83114.4037675702</v>
-      </c>
-      <c r="F82">
-        <v>1.097801573545138</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>16656.0883605474</v>
@@ -2651,16 +2153,10 @@
       <c r="D83">
         <v>1</v>
       </c>
-      <c r="E83">
-        <v>20648.7534104156</v>
-      </c>
-      <c r="F83">
-        <v>1.239712047837442</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>114644.4772193993</v>
@@ -2671,16 +2167,10 @@
       <c r="D84">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E84">
-        <v>111050.9059690918</v>
-      </c>
-      <c r="F84">
-        <v>0.9686546501195137</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>189358.7567859973</v>
@@ -2691,16 +2181,10 @@
       <c r="D85">
         <v>1</v>
       </c>
-      <c r="E85">
-        <v>175628.7397314429</v>
-      </c>
-      <c r="F85">
-        <v>0.9274920405710558</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B86">
         <v>48766.18210113559</v>
@@ -2711,16 +2195,10 @@
       <c r="D86">
         <v>1</v>
       </c>
-      <c r="E86">
-        <v>45576.1634915009</v>
-      </c>
-      <c r="F86">
-        <v>0.9345854345739235</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B87">
         <v>49163.0893981584</v>
@@ -2731,16 +2209,10 @@
       <c r="D87">
         <v>1</v>
       </c>
-      <c r="E87">
-        <v>61798.45323086721</v>
-      </c>
-      <c r="F87">
-        <v>1.257009150307428</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>340315.4048054194</v>
@@ -2751,16 +2223,10 @@
       <c r="D88">
         <v>1</v>
       </c>
-      <c r="E88">
-        <v>336273.2406020324</v>
-      </c>
-      <c r="F88">
-        <v>0.9881223002358704</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>44345.6569076197</v>
@@ -2771,16 +2237,10 @@
       <c r="D89">
         <v>1</v>
       </c>
-      <c r="E89">
-        <v>24391.2549798393</v>
-      </c>
-      <c r="F89">
-        <v>0.550025790138837</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B90">
         <v>93133.89750933739</v>
@@ -2791,16 +2251,10 @@
       <c r="D90">
         <v>1</v>
       </c>
-      <c r="E90">
-        <v>87133.6910598455</v>
-      </c>
-      <c r="F90">
-        <v>0.9355744083523367</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B91">
         <v>4224.6263586161</v>
@@ -2811,16 +2265,10 @@
       <c r="D91">
         <v>1</v>
       </c>
-      <c r="E91">
-        <v>6007.2772288846</v>
-      </c>
-      <c r="F91">
-        <v>1.42196651702293</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B92">
         <v>17974.5243846268</v>
@@ -2831,16 +2279,10 @@
       <c r="D92">
         <v>1</v>
       </c>
-      <c r="E92">
-        <v>18157.1465876633</v>
-      </c>
-      <c r="F92">
-        <v>1.010160057597557</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B93">
         <v>59618.1025332766</v>
@@ -2851,16 +2293,10 @@
       <c r="D93">
         <v>1</v>
       </c>
-      <c r="E93">
-        <v>37707.3210881244</v>
-      </c>
-      <c r="F93">
-        <v>0.6324810667544741</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B94">
         <v>97365.98607259529</v>
@@ -2871,16 +2307,10 @@
       <c r="D94">
         <v>1</v>
       </c>
-      <c r="E94">
-        <v>85194.6436588263</v>
-      </c>
-      <c r="F94">
-        <v>0.8749938977180991</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B95">
         <v>204466.887631556</v>
@@ -2891,16 +2321,10 @@
       <c r="D95">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E95">
-        <v>166184.8896946308</v>
-      </c>
-      <c r="F95">
-        <v>0.8127716503128449</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B96">
         <v>346013.9076112272</v>
@@ -2911,16 +2335,10 @@
       <c r="D96">
         <v>1</v>
       </c>
-      <c r="E96">
-        <v>286838.6011547109</v>
-      </c>
-      <c r="F96">
-        <v>0.8289799769464636</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B97">
         <v>55392.42798339461</v>
@@ -2931,16 +2349,10 @@
       <c r="D97">
         <v>1</v>
       </c>
-      <c r="E97">
-        <v>47714.8493105073</v>
-      </c>
-      <c r="F97">
-        <v>0.8613966032471284</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B98">
         <v>91239.17387506409</v>
@@ -2951,16 +2363,10 @@
       <c r="D98">
         <v>1</v>
       </c>
-      <c r="E98">
-        <v>79675.60100959719</v>
-      </c>
-      <c r="F98">
-        <v>0.8732608771611504</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B99">
         <v>1608247.583518048</v>
@@ -2971,16 +2377,10 @@
       <c r="D99">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E99">
-        <v>1506126.287399307</v>
-      </c>
-      <c r="F99">
-        <v>0.9365015081226793</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B100">
         <v>397180.3598517774</v>
@@ -2991,16 +2391,10 @@
       <c r="D100">
         <v>1</v>
       </c>
-      <c r="E100">
-        <v>491394.1503751582</v>
-      </c>
-      <c r="F100">
-        <v>1.237206569223464</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B101">
         <v>32730.400530778</v>
@@ -3011,16 +2405,10 @@
       <c r="D101">
         <v>1</v>
       </c>
-      <c r="E101">
-        <v>34494.0861422844</v>
-      </c>
-      <c r="F101">
-        <v>1.05388524377659</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B102">
         <v>47673.4401699198</v>
@@ -3031,16 +2419,10 @@
       <c r="D102">
         <v>1</v>
       </c>
-      <c r="E102">
-        <v>43050.6449823688</v>
-      </c>
-      <c r="F102">
-        <v>0.9030320620648683</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B103">
         <v>137744.3510437174</v>
@@ -3051,16 +2433,10 @@
       <c r="D103">
         <v>1</v>
       </c>
-      <c r="E103">
-        <v>115497.5119627458</v>
-      </c>
-      <c r="F103">
-        <v>0.838491822623558</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B104">
         <v>45471.80209693519</v>
@@ -3071,16 +2447,10 @@
       <c r="D104">
         <v>1</v>
       </c>
-      <c r="E104">
-        <v>40989.9130649017</v>
-      </c>
-      <c r="F104">
-        <v>0.901435860789525</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B105">
         <v>70397.1814932697</v>
@@ -3091,16 +2461,10 @@
       <c r="D105">
         <v>1</v>
       </c>
-      <c r="E105">
-        <v>57952.89357608581</v>
-      </c>
-      <c r="F105">
-        <v>0.8232274694353547</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B106">
         <v>37372.0759133016</v>
@@ -3111,16 +2475,10 @@
       <c r="D106">
         <v>1</v>
       </c>
-      <c r="E106">
-        <v>33867.0568666377</v>
-      </c>
-      <c r="F106">
-        <v>0.9062128886071222</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B107">
         <v>350133.7406666931</v>
@@ -3131,16 +2489,10 @@
       <c r="D107">
         <v>1</v>
       </c>
-      <c r="E107">
-        <v>313978.2425785799</v>
-      </c>
-      <c r="F107">
-        <v>0.8967380349598153</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B108">
         <v>561872.8047295137</v>
@@ -3151,16 +2503,10 @@
       <c r="D108">
         <v>1</v>
       </c>
-      <c r="E108">
-        <v>543079.2178158958</v>
-      </c>
-      <c r="F108">
-        <v>0.966551883708511</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B109">
         <v>246976.8807819786</v>
@@ -3171,16 +2517,10 @@
       <c r="D109">
         <v>1</v>
       </c>
-      <c r="E109">
-        <v>228799.5864455789</v>
-      </c>
-      <c r="F109">
-        <v>0.9264008263492246</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B110">
         <v>127544.7502039587</v>
@@ -3191,16 +2531,10 @@
       <c r="D110">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E110">
-        <v>150475.9615070462</v>
-      </c>
-      <c r="F110">
-        <v>1.179789534782246</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B111">
         <v>24868.1372091056</v>
@@ -3211,16 +2545,10 @@
       <c r="D111">
         <v>1</v>
       </c>
-      <c r="E111">
-        <v>39038.15505318101</v>
-      </c>
-      <c r="F111">
-        <v>1.569806162999897</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B112">
         <v>228452.0306614529</v>
@@ -3231,16 +2559,10 @@
       <c r="D112">
         <v>1</v>
       </c>
-      <c r="E112">
-        <v>471807.8000957236</v>
-      </c>
-      <c r="F112">
-        <v>2.065237935200952</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B113">
         <v>235683.5116245807</v>
@@ -3251,16 +2573,10 @@
       <c r="D113">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E113">
-        <v>247721.5897711017</v>
-      </c>
-      <c r="F113">
-        <v>1.051077303047387</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B114">
         <v>161667.5856295202</v>
@@ -3271,16 +2587,10 @@
       <c r="D114">
         <v>1</v>
       </c>
-      <c r="E114">
-        <v>162938.7045795289</v>
-      </c>
-      <c r="F114">
-        <v>1.007862546750228</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B115">
         <v>319855.6623905686</v>
@@ -3291,16 +2601,10 @@
       <c r="D115">
         <v>1</v>
       </c>
-      <c r="E115">
-        <v>270094.2681878823</v>
-      </c>
-      <c r="F115">
-        <v>0.8444254704425905</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B116">
         <v>2799289.331255021</v>
@@ -3311,67 +2615,52 @@
       <c r="D116">
         <v>1</v>
       </c>
-      <c r="E116">
-        <v>3111722.103664153</v>
-      </c>
-      <c r="F116">
-        <v>1.111611461137909</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B117">
         <v>6824</v>
       </c>
+      <c r="C117">
+        <v>6824</v>
+      </c>
       <c r="D117">
-        <v>0</v>
-      </c>
-      <c r="E117">
-        <v>6978.931580028766</v>
-      </c>
-      <c r="F117">
-        <v>1.022703924388741</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B118">
         <v>7479</v>
       </c>
+      <c r="C118">
+        <v>7479</v>
+      </c>
       <c r="D118">
-        <v>0</v>
-      </c>
-      <c r="E118">
-        <v>7648.80265050339</v>
-      </c>
-      <c r="F118">
-        <v>1.022703924388741</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B119">
         <v>8356</v>
       </c>
+      <c r="C119">
+        <v>8356</v>
+      </c>
       <c r="D119">
-        <v>0</v>
-      </c>
-      <c r="E119">
-        <v>8545.713992192315</v>
-      </c>
-      <c r="F119">
-        <v>1.02270392438874</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B120">
         <v>7361.436888645299</v>
@@ -3382,16 +2671,10 @@
       <c r="D120">
         <v>1</v>
       </c>
-      <c r="E120">
-        <v>6741.442436415</v>
-      </c>
-      <c r="F120">
-        <v>0.9157780659389182</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B121">
         <v>19358.6163389981</v>
@@ -3402,16 +2685,10 @@
       <c r="D121">
         <v>1</v>
       </c>
-      <c r="E121">
-        <v>16369.6617210497</v>
-      </c>
-      <c r="F121">
-        <v>0.8456008133222246</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B122">
         <v>43855.9940026758</v>
@@ -3422,16 +2699,10 @@
       <c r="D122">
         <v>1</v>
       </c>
-      <c r="E122">
-        <v>36280.0166023715</v>
-      </c>
-      <c r="F122">
-        <v>0.8272533191280065</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B123">
         <v>8993.438550824299</v>
@@ -3442,16 +2713,10 @@
       <c r="D123">
         <v>1</v>
       </c>
-      <c r="E123">
-        <v>7335.470580504</v>
-      </c>
-      <c r="F123">
-        <v>0.8156469340452283</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B124">
         <v>4857.0619470048</v>
@@ -3462,16 +2727,10 @@
       <c r="D124">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E124">
-        <v>3487.4750295541</v>
-      </c>
-      <c r="F124">
-        <v>0.7180215256889441</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B125">
         <v>12312.318239741</v>
@@ -3482,16 +2741,10 @@
       <c r="D125">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E125">
-        <v>12392.4150749111</v>
-      </c>
-      <c r="F125">
-        <v>1.006505422749029</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B126">
         <v>8937.525652441</v>
@@ -3502,16 +2755,10 @@
       <c r="D126">
         <v>1</v>
       </c>
-      <c r="E126">
-        <v>8521.2966951037</v>
-      </c>
-      <c r="F126">
-        <v>0.9534290615184282</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B127">
         <v>2723.7922001403</v>
@@ -3522,16 +2769,10 @@
       <c r="D127">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E127">
-        <v>1635.0202320313</v>
-      </c>
-      <c r="F127">
-        <v>0.6002734833982862</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B128">
         <v>9434.661706934699</v>
@@ -3542,16 +2783,10 @@
       <c r="D128">
         <v>1</v>
       </c>
-      <c r="E128">
-        <v>8133.6636443489</v>
-      </c>
-      <c r="F128">
-        <v>0.862104429072477</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B129">
         <v>543.1002972355</v>
@@ -3562,16 +2797,10 @@
       <c r="D129">
         <v>1</v>
       </c>
-      <c r="E129">
-        <v>217.0601571965</v>
-      </c>
-      <c r="F129">
-        <v>0.3996686400309187</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B130">
         <v>1259.8688797084</v>
@@ -3582,16 +2811,10 @@
       <c r="D130">
         <v>1</v>
       </c>
-      <c r="E130">
-        <v>1513.5217349314</v>
-      </c>
-      <c r="F130">
-        <v>1.201332741294244</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B131">
         <v>11781.071195618</v>
@@ -3602,16 +2825,10 @@
       <c r="D131">
         <v>1</v>
       </c>
-      <c r="E131">
-        <v>11824.5775878988</v>
-      </c>
-      <c r="F131">
-        <v>1.003692906320521</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B132">
         <v>819.7868429337</v>
@@ -3622,16 +2839,10 @@
       <c r="D132">
         <v>1</v>
       </c>
-      <c r="E132">
-        <v>903.5245959214001</v>
-      </c>
-      <c r="F132">
-        <v>1.102145763510957</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B133">
         <v>4412.9274828237</v>
@@ -3642,16 +2853,10 @@
       <c r="D133">
         <v>1</v>
       </c>
-      <c r="E133">
-        <v>4129.610917711</v>
-      </c>
-      <c r="F133">
-        <v>0.9357984996999283</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B134">
         <v>16300.4219503895</v>
@@ -3662,16 +2867,10 @@
       <c r="D134">
         <v>1</v>
       </c>
-      <c r="E134">
-        <v>14005.1692484127</v>
-      </c>
-      <c r="F134">
-        <v>0.8591905958654061</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B135">
         <v>7679.147481821</v>
@@ -3682,16 +2881,10 @@
       <c r="D135">
         <v>1</v>
       </c>
-      <c r="E135">
-        <v>6887.099758045</v>
-      </c>
-      <c r="F135">
-        <v>0.896857336618286</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B136">
         <v>710.3322817748</v>
@@ -3702,16 +2895,10 @@
       <c r="D136">
         <v>1</v>
       </c>
-      <c r="E136">
-        <v>489.5653593885</v>
-      </c>
-      <c r="F136">
-        <v>0.6892061250057465</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B137">
         <v>1163.6643770482</v>
@@ -3722,16 +2909,10 @@
       <c r="D137">
         <v>1</v>
       </c>
-      <c r="E137">
-        <v>1191.5298561332</v>
-      </c>
-      <c r="F137">
-        <v>1.023946319604356</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B138">
         <v>853.4575379578999</v>
@@ -3742,16 +2923,10 @@
       <c r="D138">
         <v>1</v>
       </c>
-      <c r="E138">
-        <v>549.3124514223</v>
-      </c>
-      <c r="F138">
-        <v>0.6436318469184309</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B139">
         <v>8895.3076414977</v>
@@ -3762,16 +2937,10 @@
       <c r="D139">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E139">
-        <v>9430.468749757199</v>
-      </c>
-      <c r="F139">
-        <v>1.060162180986626</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B140">
         <v>72371.27131758581</v>
@@ -3782,16 +2951,10 @@
       <c r="D140">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E140">
-        <v>57897.24929937199</v>
-      </c>
-      <c r="F140">
-        <v>0.8000032090814369</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B141">
         <v>45536.7593448985</v>
@@ -3802,16 +2965,10 @@
       <c r="D141">
         <v>1</v>
       </c>
-      <c r="E141">
-        <v>37299.26174297649</v>
-      </c>
-      <c r="F141">
-        <v>0.8191022435406383</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B142">
         <v>16488.5966841317</v>
@@ -3822,16 +2979,10 @@
       <c r="D142">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E142">
-        <v>15217.7719293585</v>
-      </c>
-      <c r="F142">
-        <v>0.9229270520033873</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B143">
         <v>9793.614960204999</v>
@@ -3842,16 +2993,10 @@
       <c r="D143">
         <v>1</v>
       </c>
-      <c r="E143">
-        <v>10152.7329934655</v>
-      </c>
-      <c r="F143">
-        <v>1.036668588128054</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B144">
         <v>10755.9041472555</v>
@@ -3862,16 +3007,10 @@
       <c r="D144">
         <v>1</v>
       </c>
-      <c r="E144">
-        <v>9583.5459994066</v>
-      </c>
-      <c r="F144">
-        <v>0.891003291606309</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B145">
         <v>3374.3120169681</v>
@@ -3882,16 +3021,10 @@
       <c r="D145">
         <v>1</v>
       </c>
-      <c r="E145">
-        <v>3442.2936337921</v>
-      </c>
-      <c r="F145">
-        <v>1.020146808144045</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B146">
         <v>33280.2929776912</v>
@@ -3902,16 +3035,10 @@
       <c r="D146">
         <v>1</v>
       </c>
-      <c r="E146">
-        <v>29057.0060947669</v>
-      </c>
-      <c r="F146">
-        <v>0.8730994680318681</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B147">
         <v>11756.3612042058</v>
@@ -3922,16 +3049,10 @@
       <c r="D147">
         <v>1</v>
       </c>
-      <c r="E147">
-        <v>12343.8126677245</v>
-      </c>
-      <c r="F147">
-        <v>1.049968817163302</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B148">
         <v>6261.775489857901</v>
@@ -3942,16 +3063,10 @@
       <c r="D148">
         <v>1</v>
       </c>
-      <c r="E148">
-        <v>5758.6335682834</v>
-      </c>
-      <c r="F148">
-        <v>0.9196486807312987</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6">
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B149">
         <v>1661.2077547693</v>
@@ -3962,16 +3077,10 @@
       <c r="D149">
         <v>1</v>
       </c>
-      <c r="E149">
-        <v>1083.2302652926</v>
-      </c>
-      <c r="F149">
-        <v>0.6520739276485219</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B150">
         <v>389.6873722863</v>
@@ -3982,16 +3091,10 @@
       <c r="D150">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E150">
-        <v>494.1755741925</v>
-      </c>
-      <c r="F150">
-        <v>1.268133404716623</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B151">
         <v>3298.5137005144</v>
@@ -4002,16 +3105,10 @@
       <c r="D151">
         <v>1</v>
       </c>
-      <c r="E151">
-        <v>3289.175204330299</v>
-      </c>
-      <c r="F151">
-        <v>0.9971688775515335</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B152">
         <v>4925.2072663299</v>
@@ -4022,16 +3119,10 @@
       <c r="D152">
         <v>1</v>
       </c>
-      <c r="E152">
-        <v>4288.4323643019</v>
-      </c>
-      <c r="F152">
-        <v>0.8707110447145703</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B153">
         <v>2913.0855896192</v>
@@ -4042,16 +3133,10 @@
       <c r="D153">
         <v>1</v>
       </c>
-      <c r="E153">
-        <v>3722.3597896504</v>
-      </c>
-      <c r="F153">
-        <v>1.277806530269846</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B154">
         <v>21549.0073335034</v>
@@ -4062,16 +3147,10 @@
       <c r="D154">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E154">
-        <v>21616.8713012093</v>
-      </c>
-      <c r="F154">
-        <v>1.003149285099569</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B155">
         <v>15594.1131265109</v>
@@ -4082,16 +3161,10 @@
       <c r="D155">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E155">
-        <v>16088.1616787959</v>
-      </c>
-      <c r="F155">
-        <v>1.031681734528723</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B156">
         <v>26214.2213800131</v>
@@ -4102,16 +3175,10 @@
       <c r="D156">
         <v>1</v>
       </c>
-      <c r="E156">
-        <v>21218.9263627885</v>
-      </c>
-      <c r="F156">
-        <v>0.8094433191506792</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B157">
         <v>6600.5918929203</v>
@@ -4122,16 +3189,10 @@
       <c r="D157">
         <v>1</v>
       </c>
-      <c r="E157">
-        <v>5162.177482816601</v>
-      </c>
-      <c r="F157">
-        <v>0.7820779661220197</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6">
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B158">
         <v>17517.2789309422</v>
@@ -4142,16 +3203,10 @@
       <c r="D158">
         <v>1</v>
       </c>
-      <c r="E158">
-        <v>17060.3957771812</v>
-      </c>
-      <c r="F158">
-        <v>0.9739181435905566</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6">
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B159">
         <v>6630.1085138655</v>
@@ -4162,16 +3217,10 @@
       <c r="D159">
         <v>1</v>
       </c>
-      <c r="E159">
-        <v>7487.7831975187</v>
-      </c>
-      <c r="F159">
-        <v>1.129360580126185</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6">
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B160">
         <v>6683.812627174399</v>
@@ -4182,16 +3231,10 @@
       <c r="D160">
         <v>1</v>
       </c>
-      <c r="E160">
-        <v>6520.18595491</v>
-      </c>
-      <c r="F160">
-        <v>0.9755189617974714</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6">
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B161">
         <v>7364.364875575</v>
@@ -4202,16 +3245,10 @@
       <c r="D161">
         <v>1</v>
       </c>
-      <c r="E161">
-        <v>8198.289279941599</v>
-      </c>
-      <c r="F161">
-        <v>1.113237790149756</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B162">
         <v>7505.2364324431</v>
@@ -4222,16 +3259,10 @@
       <c r="D162">
         <v>1</v>
       </c>
-      <c r="E162">
-        <v>8691.654805009699</v>
-      </c>
-      <c r="F162">
-        <v>1.158078747184837</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B163">
         <v>4518.674197097101</v>
@@ -4242,16 +3273,10 @@
       <c r="D163">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E163">
-        <v>5109.0523263543</v>
-      </c>
-      <c r="F163">
-        <v>1.13065295338984</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B164">
         <v>1940.546519116</v>
@@ -4262,16 +3287,10 @@
       <c r="D164">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E164">
-        <v>2059.2923423997</v>
-      </c>
-      <c r="F164">
-        <v>1.06119194882161</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6">
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B165">
         <v>2544.1929848693</v>
@@ -4282,16 +3301,10 @@
       <c r="D165">
         <v>1</v>
       </c>
-      <c r="E165">
-        <v>1995.1892644401</v>
-      </c>
-      <c r="F165">
-        <v>0.7842130201229985</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6">
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B166">
         <v>16417.2059842253</v>
@@ -4302,16 +3315,10 @@
       <c r="D166">
         <v>1</v>
       </c>
-      <c r="E166">
-        <v>14200.8338211036</v>
-      </c>
-      <c r="F166">
-        <v>0.8649969936875171</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6">
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B167">
         <v>6021.122840665499</v>
@@ -4322,16 +3329,10 @@
       <c r="D167">
         <v>1</v>
       </c>
-      <c r="E167">
-        <v>5582.6857759808</v>
-      </c>
-      <c r="F167">
-        <v>0.9271835044248591</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B168">
         <v>8042.143418413099</v>
@@ -4342,16 +3343,10 @@
       <c r="D168">
         <v>1</v>
       </c>
-      <c r="E168">
-        <v>7723.7464210512</v>
-      </c>
-      <c r="F168">
-        <v>0.9604089381653024</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6">
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B169">
         <v>14635.054526756</v>
@@ -4362,16 +3357,10 @@
       <c r="D169">
         <v>1</v>
       </c>
-      <c r="E169">
-        <v>14723.8570528076</v>
-      </c>
-      <c r="F169">
-        <v>1.006067796050179</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6">
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B170">
         <v>3922.2244164923</v>
@@ -4382,16 +3371,10 @@
       <c r="D170">
         <v>1</v>
       </c>
-      <c r="E170">
-        <v>3679.7845200637</v>
-      </c>
-      <c r="F170">
-        <v>0.9381881629696708</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6">
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B171">
         <v>16345.7540730271</v>
@@ -4402,16 +3385,10 @@
       <c r="D171">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E171">
-        <v>18559.8453181616</v>
-      </c>
-      <c r="F171">
-        <v>1.135453600686925</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6">
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B172">
         <v>6225.6638480783</v>
@@ -4422,16 +3399,10 @@
       <c r="D172">
         <v>1</v>
       </c>
-      <c r="E172">
-        <v>6459.7748513545</v>
-      </c>
-      <c r="F172">
-        <v>1.037604183102251</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6">
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B173">
         <v>559.551440978</v>
@@ -4442,16 +3413,10 @@
       <c r="D173">
         <v>1</v>
       </c>
-      <c r="E173">
-        <v>505.0709031335</v>
-      </c>
-      <c r="F173">
-        <v>0.9026353363521371</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6">
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B174">
         <v>22665.7517510057</v>
@@ -4462,16 +3427,10 @@
       <c r="D174">
         <v>1</v>
       </c>
-      <c r="E174">
-        <v>22393.0965411748</v>
-      </c>
-      <c r="F174">
-        <v>0.987970608130445</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6">
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B175">
         <v>632.9046643452</v>
@@ -4482,16 +3441,10 @@
       <c r="D175">
         <v>1</v>
       </c>
-      <c r="E175">
-        <v>972.7048793333</v>
-      </c>
-      <c r="F175">
-        <v>1.536890047002033</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6">
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B176">
         <v>12359.8393763968</v>
@@ -4502,16 +3455,10 @@
       <c r="D176">
         <v>1</v>
       </c>
-      <c r="E176">
-        <v>10382.2676063193</v>
-      </c>
-      <c r="F176">
-        <v>0.8400002047070282</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6">
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B177">
         <v>32557.6112073765</v>
@@ -4522,16 +3469,10 @@
       <c r="D177">
         <v>1</v>
       </c>
-      <c r="E177">
-        <v>25699.6463856599</v>
-      </c>
-      <c r="F177">
-        <v>0.7893590909346935</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6">
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B178">
         <v>8567.277724928001</v>
@@ -4542,16 +3483,10 @@
       <c r="D178">
         <v>0.9999999999999998</v>
       </c>
-      <c r="E178">
-        <v>9038.789579808701</v>
-      </c>
-      <c r="F178">
-        <v>1.055036368613189</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B179">
         <v>10350.506824964</v>
@@ -4562,16 +3497,10 @@
       <c r="D179">
         <v>1</v>
       </c>
-      <c r="E179">
-        <v>7923.416704286001</v>
-      </c>
-      <c r="F179">
-        <v>0.7655100217098363</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B180">
         <v>4516.030838189</v>
@@ -4582,16 +3511,10 @@
       <c r="D180">
         <v>1</v>
       </c>
-      <c r="E180">
-        <v>4585.076875446901</v>
-      </c>
-      <c r="F180">
-        <v>1.015289097823253</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6">
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B181">
         <v>1518.0251162358</v>
@@ -4602,16 +3525,10 @@
       <c r="D181">
         <v>1</v>
       </c>
-      <c r="E181">
-        <v>1263.2202501748</v>
-      </c>
-      <c r="F181">
-        <v>0.8321471342365983</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6">
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B182">
         <v>9014.747951125899</v>
@@ -4622,16 +3539,10 @@
       <c r="D182">
         <v>1</v>
       </c>
-      <c r="E182">
-        <v>8891.793361173999</v>
-      </c>
-      <c r="F182">
-        <v>0.9863607290388475</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6">
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B183">
         <v>6586.2585662836</v>
@@ -4642,16 +3553,10 @@
       <c r="D183">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E183">
-        <v>6329.4764074702</v>
-      </c>
-      <c r="F183">
-        <v>0.9610124388180081</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6">
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B184">
         <v>8602.8882684122</v>
@@ -4662,16 +3567,10 @@
       <c r="D184">
         <v>1</v>
       </c>
-      <c r="E184">
-        <v>8841.8388134181</v>
-      </c>
-      <c r="F184">
-        <v>1.027775618786457</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6">
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B185">
         <v>620.3568502964999</v>
@@ -4682,16 +3581,10 @@
       <c r="D185">
         <v>1</v>
       </c>
-      <c r="E185">
-        <v>456.7162020974</v>
-      </c>
-      <c r="F185">
-        <v>0.7362152958883459</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6">
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B186">
         <v>954.6886864584</v>
@@ -4702,16 +3595,10 @@
       <c r="D186">
         <v>1</v>
       </c>
-      <c r="E186">
-        <v>781.8063005051</v>
-      </c>
-      <c r="F186">
-        <v>0.818912292137199</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6">
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B187">
         <v>1656.0729215435</v>
@@ -4722,16 +3609,10 @@
       <c r="D187">
         <v>1</v>
       </c>
-      <c r="E187">
-        <v>1108.9937547332</v>
-      </c>
-      <c r="F187">
-        <v>0.6696527310521997</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6">
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B188">
         <v>137590.542329113</v>
@@ -4742,16 +3623,10 @@
       <c r="D188">
         <v>1</v>
       </c>
-      <c r="E188">
-        <v>127704.1886885103</v>
-      </c>
-      <c r="F188">
-        <v>0.9281465609972319</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6">
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B189">
         <v>97022.56059828011</v>
@@ -4762,16 +3637,10 @@
       <c r="D189">
         <v>1</v>
       </c>
-      <c r="E189">
-        <v>81696.6651529927</v>
-      </c>
-      <c r="F189">
-        <v>0.8420378172789733</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6">
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B190">
         <v>3709.051398008</v>
@@ -4782,16 +3651,10 @@
       <c r="D190">
         <v>1</v>
       </c>
-      <c r="E190">
-        <v>2826.7138655195</v>
-      </c>
-      <c r="F190">
-        <v>0.762112346849016</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6">
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B191">
         <v>48369.13837138349</v>
@@ -4802,16 +3665,10 @@
       <c r="D191">
         <v>0.9999999999999999</v>
       </c>
-      <c r="E191">
-        <v>38833.544943546</v>
-      </c>
-      <c r="F191">
-        <v>0.8028579017756701</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6">
+    </row>
+    <row r="192" spans="1:4">
       <c r="A192" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B192">
         <v>666.8205317435999</v>
@@ -4822,16 +3679,10 @@
       <c r="D192">
         <v>1</v>
       </c>
-      <c r="E192">
-        <v>636.3012318894999</v>
-      </c>
-      <c r="F192">
-        <v>0.9542316134533257</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6">
+    </row>
+    <row r="193" spans="1:4">
       <c r="A193" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B193">
         <v>1615.3490763407</v>
@@ -4842,16 +3693,10 @@
       <c r="D193">
         <v>1</v>
       </c>
-      <c r="E193">
-        <v>1576.0261988335</v>
-      </c>
-      <c r="F193">
-        <v>0.975656730744367</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6">
+    </row>
+    <row r="194" spans="1:4">
       <c r="A194" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B194">
         <v>840.9189392032</v>
@@ -4862,16 +3707,10 @@
       <c r="D194">
         <v>1</v>
       </c>
-      <c r="E194">
-        <v>1023.1021001239</v>
-      </c>
-      <c r="F194">
-        <v>1.216647708152851</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6">
+    </row>
+    <row r="195" spans="1:4">
       <c r="A195" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B195">
         <v>43174.3571289298</v>
@@ -4882,16 +3721,10 @@
       <c r="D195">
         <v>1</v>
       </c>
-      <c r="E195">
-        <v>40026.8221559277</v>
-      </c>
-      <c r="F195">
-        <v>0.9270971200890672</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6">
+    </row>
+    <row r="196" spans="1:4">
       <c r="A196" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B196">
         <v>29910.7076361184</v>
@@ -4902,16 +3735,10 @@
       <c r="D196">
         <v>1</v>
       </c>
-      <c r="E196">
-        <v>35969.2382899906</v>
-      </c>
-      <c r="F196">
-        <v>1.202553905697513</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6">
+    </row>
+    <row r="197" spans="1:4">
       <c r="A197" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B197">
         <v>734181.2608958975</v>
@@ -4922,16 +3749,10 @@
       <c r="D197">
         <v>0.9999999999999997</v>
       </c>
-      <c r="E197">
-        <v>637526.821849563</v>
-      </c>
-      <c r="F197">
-        <v>0.8683507136529334</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6">
+    </row>
+    <row r="198" spans="1:4">
       <c r="A198" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B198">
         <v>164552.0289146891</v>
@@ -4942,106 +3763,85 @@
       <c r="D198">
         <v>1</v>
       </c>
-      <c r="E198">
-        <v>253757.1642389746</v>
-      </c>
-      <c r="F198">
-        <v>1.542108996848245</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6">
+    </row>
+    <row r="199" spans="1:4">
       <c r="A199" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B199">
         <v>80477.5230836588</v>
       </c>
+      <c r="C199">
+        <v>80477.52308365879</v>
+      </c>
       <c r="D199">
-        <v>0</v>
-      </c>
-      <c r="E199">
-        <v>82304.6786827433</v>
-      </c>
-      <c r="F199">
-        <v>1.02270392438874</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6">
+        <v>0.9999999999999998</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
       <c r="A200" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B200">
         <v>130773.8788847713</v>
       </c>
+      <c r="C200">
+        <v>130773.8788847713</v>
+      </c>
       <c r="D200">
-        <v>0</v>
-      </c>
-      <c r="E200">
-        <v>133742.9591429935</v>
-      </c>
-      <c r="F200">
-        <v>1.022703924388741</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
       <c r="A201" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B201">
         <v>130773.8788847713</v>
       </c>
+      <c r="C201">
+        <v>130773.8788847713</v>
+      </c>
       <c r="D201">
-        <v>0</v>
-      </c>
-      <c r="E201">
-        <v>133742.9591429935</v>
-      </c>
-      <c r="F201">
-        <v>1.022703924388741</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
       <c r="A202" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B202">
         <v>4023589.873533676</v>
       </c>
+      <c r="C202">
+        <v>4023589.873533676</v>
+      </c>
       <c r="D202">
-        <v>0</v>
-      </c>
-      <c r="E202">
-        <v>4114941.153793687</v>
-      </c>
-      <c r="F202">
-        <v>1.022703924388741</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
       <c r="A203" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B203">
         <v>40641624.89898051</v>
       </c>
+      <c r="C203">
+        <v>40641624.89898051</v>
+      </c>
       <c r="D203">
-        <v>0</v>
-      </c>
-      <c r="E203">
-        <v>41564349.27772252</v>
-      </c>
-      <c r="F203">
-        <v>1.022703924388741</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
       <c r="A204" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B204">
         <v>0</v>
       </c>
-      <c r="E204">
+      <c r="C204">
         <v>0</v>
       </c>
     </row>

</xml_diff>